<commit_message>
Policy Fixes and adding What's New
</commit_message>
<xml_diff>
--- a/docs/content/policy/policyAssignments/data/ALZPolicyAssignments.xlsx
+++ b/docs/content/policy/policyAssignments/data/ALZPolicyAssignments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10125"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/springstone/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/springstone/repos/Springstone/Azure-Landing-Zones/docs/content/policy/policyAssignments/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6601C325-E8A7-FC49-A181-206B447BDAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D7D3D7-E22C-7844-B666-E29A8C1A4F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="430">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -1300,9 +1300,6 @@
     <t>DINE-ServiceHealthBuiltInPolicyAssignment.json</t>
   </si>
   <si>
-    <t>[Preview]: Configure subscriptions to enable service health alert monitoring rule - 98903777-a9f6-47f5-90a9-acaf62ab01a8 Azure Policy</t>
-  </si>
-  <si>
     <t>FY25H2</t>
   </si>
   <si>
@@ -1319,6 +1316,12 @@
   </si>
   <si>
     <t>https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e3ec7e09-768c-4b64-882c-fcada3772047.html</t>
+  </si>
+  <si>
+    <t>Enforce-Backup</t>
+  </si>
+  <si>
+    <t>Updated 260203</t>
   </si>
 </sst>
 </file>
@@ -1946,9 +1949,9 @@
   </sheetPr>
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2168,10 +2171,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>11</v>
@@ -2180,16 +2183,16 @@
         <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J7" s="6">
         <v>45992</v>
@@ -2508,7 +2511,9 @@
       <c r="H17" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="J17" s="6">
         <v>45427</v>
       </c>
@@ -2539,11 +2544,11 @@
       <c r="H18" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>422</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>423</v>
       </c>
       <c r="K18" s="3"/>
     </row>
@@ -2578,6 +2583,9 @@
       <c r="J19" s="6">
         <v>45124</v>
       </c>
+      <c r="K19" s="1" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="20" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -2604,7 +2612,9 @@
       <c r="H20" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="J20" s="6">
         <v>45363</v>
       </c>
@@ -2993,7 +3003,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -3025,7 +3035,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="1" customFormat="1" ht="128" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="1" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>57</v>
       </c>
@@ -3057,7 +3067,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -3089,7 +3099,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -3121,7 +3131,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -3153,7 +3163,7 @@
         <v>45084</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -3185,7 +3195,7 @@
         <v>45084</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -3217,7 +3227,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -3249,7 +3259,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -3281,7 +3291,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -3313,7 +3323,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -3344,8 +3354,11 @@
       <c r="J43" s="6">
         <v>45018</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="K43" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -3370,12 +3383,14 @@
       <c r="H44" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I44" s="4"/>
+      <c r="I44" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="J44" s="6">
         <v>45363</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -3407,7 +3422,7 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -3439,7 +3454,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -3471,7 +3486,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -4391,9 +4406,12 @@
     <hyperlink ref="I74" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/281d9e47-d14d-4f05-b8eb-18f2c4a034ff.html" xr:uid="{D206ECB8-9E61-4E32-80CA-0DDF0C03A46F}"/>
     <hyperlink ref="I75" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/281d9e47-d14d-4f05-b8eb-18f2c4a034ff.html" xr:uid="{FCEA4117-D58D-47F6-A527-0F43A12942BA}"/>
     <hyperlink ref="I18" r:id="rId3" display="https://www.azadvertizer.net/azpolicyadvertizer/98903777-a9f6-47f5-90a9-acaf62ab01a8.html" xr:uid="{B8DC5C77-1DEC-44D7-B886-FC7EFCCA2B3B}"/>
+    <hyperlink ref="I20" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Backup.html" xr:uid="{3AC2730F-D716-C749-A3AD-3A407EC21168}"/>
+    <hyperlink ref="I17" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-TrustedLaunch.html" xr:uid="{A150D68D-B343-2D49-BC3E-23415CE75C99}"/>
+    <hyperlink ref="I44" r:id="rId6" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Backup.html" xr:uid="{BD6915F6-A1CF-C74F-A4CF-A8C57364E736}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -5617,28 +5635,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29d6274d96300b72dcb696c613f494d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a8542fb098e640cc25653cbc1ecb0f8e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5916,10 +5912,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72C5CC99-3819-4588-BB45-481593D3932B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9795881-6E33-4D17-9FF0-21053BCB75EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5943,21 +5973,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9795881-6E33-4D17-9FF0-21053BCB75EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72C5CC99-3819-4588-BB45-481593D3932B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>